<commit_message>
script now writing to destination excel file. Next step: reading attachment contents
</commit_message>
<xml_diff>
--- a/end/dest.xlsx
+++ b/end/dest.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\addis\Documents\waterfleet\dadps\end\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\addis\GitHub\Outlook-Excel-PowerShell\end\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>Date</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Test Field #1</t>
   </si>
@@ -353,10 +350,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A3:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -364,24 +361,19 @@
     <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Script saves unread messages of specified subject and attachment name to pre-created excel file. Creates and destroys temporary text files when transferring contents to excel destination
</commit_message>
<xml_diff>
--- a/end/dest.xlsx
+++ b/end/dest.xlsx
@@ -24,15 +24,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>Test Field #1</t>
-  </si>
-  <si>
-    <t>Test Field #2</t>
-  </si>
-  <si>
-    <t>Test Field #3</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
+  <si>
+    <t xml:space="preserve">This is a heading. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">More details. Test # 1. </t>
+  </si>
+  <si>
+    <t>Test Field #1: 204.33</t>
+  </si>
+  <si>
+    <t>Test Field #2: 201.23231</t>
+  </si>
+  <si>
+    <t>Test Field #3: 701.9</t>
+  </si>
+  <si>
+    <t>#22222222222222</t>
   </si>
 </sst>
 </file>
@@ -350,10 +359,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:A5"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="F8" sqref="A1:F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -361,19 +370,52 @@
     <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
script now only writes data to excel sheet
</commit_message>
<xml_diff>
--- a/end/dest.xlsx
+++ b/end/dest.xlsx
@@ -24,24 +24,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>#22222222222222</t>
+  </si>
   <si>
     <t xml:space="preserve">This is a heading. </t>
   </si>
   <si>
     <t xml:space="preserve">More details. Test # 1. </t>
-  </si>
-  <si>
-    <t>Test Field #1: 204.33</t>
-  </si>
-  <si>
-    <t>Test Field #2: 201.23231</t>
-  </si>
-  <si>
-    <t>Test Field #3: 701.9</t>
-  </si>
-  <si>
-    <t>#22222222222222</t>
   </si>
 </sst>
 </file>
@@ -359,10 +350,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="A1:F8"/>
+      <selection activeCell="C8" sqref="A1:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -370,52 +361,34 @@
     <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
         <v>2</v>
       </c>
-      <c r="B6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" t="s">
-        <v>4</v>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>204.33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>201.23231000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>701.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added date email sent to the top of each row, attachment row data split after : read in as double if number, else read as string
</commit_message>
<xml_diff>
--- a/end/dest.xlsx
+++ b/end/dest.xlsx
@@ -24,15 +24,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>#22222222222222</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="3">
   <si>
     <t xml:space="preserve">This is a heading. </t>
   </si>
   <si>
     <t xml:space="preserve">More details. Test # 1. </t>
+  </si>
+  <si>
+    <t>#22222222222222</t>
   </si>
 </sst>
 </file>
@@ -68,8 +68,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -350,44 +351,72 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="A1:C8"/>
+      <selection activeCell="C10" sqref="A1:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1">
+        <v>42289.739444444444</v>
+      </c>
+      <c r="B1" s="1">
+        <v>42299.564837962964</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>204.33</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>201.23231000000001</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+        <v>201.23</v>
+      </c>
+      <c r="B7">
+        <v>204.33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
+        <v>701.9</v>
+      </c>
+      <c r="B8">
+        <v>201.23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9">
         <v>701.9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
allows printing for Date and Time rows, allows data as 0 to print, casts Time in military format to DateTime before printing
</commit_message>
<xml_diff>
--- a/end/dest.xlsx
+++ b/end/dest.xlsx
@@ -24,15 +24,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="2">
   <si>
-    <t xml:space="preserve">This is a heading. </t>
+    <t xml:space="preserve">	11 / 12 / 2015</t>
   </si>
   <si>
-    <t xml:space="preserve">More details. Test # 1. </t>
-  </si>
-  <si>
-    <t>#22222222222222</t>
+    <t xml:space="preserve">	10 / 12 / 2015</t>
   </si>
 </sst>
 </file>
@@ -70,7 +67,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -351,73 +348,435 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="A1:C10"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="I11" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="2" max="3" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1">
-        <v>42289.739444444444</v>
-      </c>
-      <c r="B1" s="1">
-        <v>42299.564837962964</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.2638888888888889</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0.63888888888888895</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>31</v>
+      </c>
+      <c r="D3">
+        <v>31</v>
+      </c>
+      <c r="E3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>34.74</v>
+      </c>
+      <c r="D4">
+        <v>34.74</v>
+      </c>
+      <c r="E4">
+        <v>34.74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>204.33</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>28.32</v>
+      </c>
+      <c r="D5">
+        <v>28.32</v>
+      </c>
+      <c r="E5">
+        <v>28.32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
+        <v>201.23</v>
+      </c>
+      <c r="B6">
         <v>204.33</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>126.48</v>
+      </c>
+      <c r="D6">
+        <v>126.48</v>
+      </c>
+      <c r="E6">
+        <v>126.48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
+        <v>701.9</v>
+      </c>
+      <c r="B7">
         <v>201.23</v>
       </c>
-      <c r="B7">
-        <v>204.33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8">
         <v>701.9</v>
       </c>
-      <c r="B8">
-        <v>201.23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B9">
-        <v>701.9</v>
+      <c r="C8">
+        <v>102.09</v>
+      </c>
+      <c r="D8">
+        <v>102.09</v>
+      </c>
+      <c r="E8">
+        <v>102.09</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>868.85</v>
+      </c>
+      <c r="D9">
+        <v>868.85</v>
+      </c>
+      <c r="E9">
+        <v>868.85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>58.04</v>
+      </c>
+      <c r="D10">
+        <v>58.04</v>
+      </c>
+      <c r="E10">
+        <v>58.04</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>55.83</v>
+      </c>
+      <c r="D11">
+        <v>55.83</v>
+      </c>
+      <c r="E11">
+        <v>55.83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>50.14</v>
+      </c>
+      <c r="D12">
+        <v>50.14</v>
+      </c>
+      <c r="E12">
+        <v>50.14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <v>46.65</v>
+      </c>
+      <c r="D13">
+        <v>46.65</v>
+      </c>
+      <c r="E13">
+        <v>46.65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <v>40.94</v>
+      </c>
+      <c r="D14">
+        <v>40.94</v>
+      </c>
+      <c r="E14">
+        <v>40.94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <v>180.66</v>
+      </c>
+      <c r="D15">
+        <v>180.66</v>
+      </c>
+      <c r="E15">
+        <v>180.66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <v>3.69</v>
+      </c>
+      <c r="D16">
+        <v>3.69</v>
+      </c>
+      <c r="E16">
+        <v>3.69</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <v>12.51</v>
+      </c>
+      <c r="D17">
+        <v>12.51</v>
+      </c>
+      <c r="E17">
+        <v>12.51</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="D18">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="E18">
+        <v>18.100000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C19">
+        <v>7.45</v>
+      </c>
+      <c r="D19">
+        <v>7.45</v>
+      </c>
+      <c r="E19">
+        <v>7.45</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="D20">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="E20">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="21" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <v>7.53</v>
+      </c>
+      <c r="D21">
+        <v>7.53</v>
+      </c>
+      <c r="E21">
+        <v>7.53</v>
+      </c>
+    </row>
+    <row r="22" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <v>1416.56</v>
+      </c>
+      <c r="D22">
+        <v>1416.56</v>
+      </c>
+      <c r="E22">
+        <v>1416.56</v>
+      </c>
+    </row>
+    <row r="23" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C23">
+        <v>29.08</v>
+      </c>
+      <c r="D23">
+        <v>29.08</v>
+      </c>
+      <c r="E23">
+        <v>29.08</v>
+      </c>
+    </row>
+    <row r="24" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C24">
+        <v>33.75</v>
+      </c>
+      <c r="D24">
+        <v>33.75</v>
+      </c>
+      <c r="E24">
+        <v>33.75</v>
+      </c>
+    </row>
+    <row r="25" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C25">
+        <v>642.20000000000005</v>
+      </c>
+      <c r="D25">
+        <v>642.20000000000005</v>
+      </c>
+      <c r="E25">
+        <v>642.20000000000005</v>
+      </c>
+    </row>
+    <row r="26" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C26">
+        <v>159839</v>
+      </c>
+      <c r="D26">
+        <v>159839</v>
+      </c>
+      <c r="E26">
+        <v>159839</v>
+      </c>
+    </row>
+    <row r="27" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C27">
+        <v>73.22</v>
+      </c>
+      <c r="D27">
+        <v>73.22</v>
+      </c>
+      <c r="E27">
+        <v>73.22</v>
+      </c>
+    </row>
+    <row r="28" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C28">
+        <v>30.86</v>
+      </c>
+      <c r="D28">
+        <v>30.86</v>
+      </c>
+      <c r="E28">
+        <v>30.86</v>
+      </c>
+    </row>
+    <row r="29" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C29">
+        <v>130791</v>
+      </c>
+      <c r="D29">
+        <v>130791</v>
+      </c>
+      <c r="E29">
+        <v>130791</v>
+      </c>
+    </row>
+    <row r="30" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>